<commit_message>
Ran three test cases updated spreadsheet with results. Filled out defect log with the two defects found from testing.
</commit_message>
<xml_diff>
--- a/docs/formal/Defect_Log_V1.xlsx
+++ b/docs/formal/Defect_Log_V1.xlsx
@@ -5,26 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert Norwood\Desktop\portfolioProjs\envogueGrooming\docs\formal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67588B10-BF5F-45BF-8D3F-3B4FF153F22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472F9766-211F-49A0-B362-0C3B8850AFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15890" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Log" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Defect Log'!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Defect ID</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>DEF-001</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -108,13 +105,103 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>DEF-001-NOTIF-001</t>
+  </si>
+  <si>
+    <t>SMS confirmation not delivered due to unverified toll-free sender</t>
+  </si>
+  <si>
+    <t>Booking confirmation SMS is successfully sent via Twilio API and recorded as smsStatus = "Sent" in the database; however, the message is not delivered to the recipient phone number. Twilio Messaging Logs show the message as Undelivered when sent from an unverified toll-free number.</t>
+  </si>
+  <si>
+    <t>Create a booking with a valid payload
+Use verified recipient phone number
+Observe Twilio Messaging Logs</t>
+  </si>
+  <si>
+    <t>Customer receives SMS confirmation.</t>
+  </si>
+  <si>
+    <t>Twilio API accepts request, but carriers block delivery due to toll-free verification requirements.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>External carrier compliance (A2P/10DLC / Toll-Free Verification) required by Twilio for SMS delivery.</t>
+  </si>
+  <si>
+    <t>Robert Norwood</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>DEF-002-NOTIF-002</t>
+  </si>
+  <si>
+    <t>Booking smsStatus reflects send request accepted, not final delivery outcome</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Booking Notifications</t>
+  </si>
+  <si>
+    <t>Root Cause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Workaround</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Use Twilio Virtual Phone for testing or verify toll-free sender / switch to local long-code number.</t>
+  </si>
+  <si>
+    <t>When SMS delivery ultimately fails (e.g., unverified recipient / carrier blocking), Twilio Messaging Logs show failed/undelivered, but the Booking record remains smsStatus = "Sent" because the app only updates status based on the immediate messages.create() response. Final delivery receipts are asynchronous and require Twilio statusCallback webhook to reconcile.</t>
+  </si>
+  <si>
+    <t>Use Twilio Messaging Logs as source of truth for delivery during V1 testing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Twilio statusCallback webhook and store smsMessageSid to update booking status asynchronously, in V2 of project. </t>
+  </si>
+  <si>
+    <t>Ensure the application is running in the Development environment with Twilio configured. Using Postman, send a POST /api/bookings request with a valid serviceId, an available date and time, and a phone number that will ultimately fail delivery (e.g., an unverified number or a carrier-blocked number). Submit the request and observe that the API returns HTTP 201 Created and the booking is created successfully. Check the booking record in the database and observe that smsStatus is set to “Sent” and smsError is empty. Navigate to the Twilio Console under Messaging Logs, locate the corresponding message, and observe that Twilio reports the message status as Failed or Undelivered.</t>
+  </si>
+  <si>
+    <t>Booking is created successfully with status = "Confirmed".
+Application sets smsStatus = "Sent" because the Twilio API accepted the send request.
+Twilio Messaging Logs later show the message as Failed/Undelivered.
+Database does not reflect the final delivery failure.</t>
+  </si>
+  <si>
+    <t>Booking record reflects the final delivery outcome of the SMS (e.g., smsStatus = "Failed" when Twilio marks the message as failed).</t>
+  </si>
+  <si>
+    <t>SMS delivery status is asynchronous.
+The current implementation updates smsStatus based only on the immediate response from client.messages.create() (provider acceptance), not the final carrier delivery result.
+Twilio provides final delivery states (failed, undelivered, delivered) after the initial request via status callback webhooks, which are not implemented in V1.
+As a result:
+The application correctly records provider acceptance.
+Final delivery failures occurring downstream are not reconciled back to the booking record.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +219,19 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -174,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -182,6 +282,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,80 +591,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="3" customWidth="1"/>
-    <col min="3" max="4" width="36" style="3" customWidth="1"/>
-    <col min="5" max="6" width="30" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36" style="3" customWidth="1"/>
+    <col min="5" max="5" width="82.42578125" style="3" customWidth="1"/>
+    <col min="6" max="9" width="30" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="4">
+        <v>46042</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="360" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="4">
+        <v>46042</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -567,19 +914,19 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1000</xm:sqref>
+          <xm:sqref>L2:L1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1000</xm:sqref>
+          <xm:sqref>J2:J1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1000</xm:sqref>
+          <xm:sqref>K2:K1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -608,51 +955,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>